<commit_message>
Mise en place rapport d'optimisation
</commit_message>
<xml_diff>
--- a/Audit-SEO (LA CHOUETTE AGENCE).xlsx
+++ b/Audit-SEO (LA CHOUETTE AGENCE).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Catégorie</t>
   </si>
@@ -116,13 +116,32 @@
     <t xml:space="preserve">Robots.text n'est pas set </t>
   </si>
   <si>
+    <t>Si les pages ne sont pas autorisées à parcourir le fichier robots.txt, aucune information sur l'indexation ou la diffusion des directives ne sera trouvée et sera donc ignorée.​</t>
+  </si>
+  <si>
+    <t>Ajouter les en-têtes HTTP X-Robots-Tag</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lien Cannonique inéxistant </t>
   </si>
   <si>
     <t>Les descriptions images ne sont pas bonnes</t>
   </si>
   <si>
+    <t xml:space="preserve">Le texte alternatif  doit présenté le contenu ou la fonction d'une image aux utilisateurs de lecteurs d'écran ou dans d'autres situations où les images ne peuvent être vues ou ne sont pas disponibles.
+</t>
+  </si>
+  <si>
+    <t>Assurez-vous que le texte alternatif transmet le contenu et la fonction de l'image de manière précise et succincte. L'attribut alt doit être équivalent, précis et succinct.</t>
+  </si>
+  <si>
     <t>Le titre de la page n'est  pas présent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le titre de la page est "." </t>
+  </si>
+  <si>
+    <t>Minifier code Css</t>
   </si>
 </sst>
 </file>
@@ -158,16 +177,15 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="-apple-system"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="&quot;Open Sans&quot;"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +204,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -199,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -224,20 +248,38 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +551,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -545,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="6"/>
@@ -583,7 +625,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="6"/>
@@ -621,7 +663,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="6"/>
@@ -659,7 +701,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -695,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="6"/>
@@ -729,7 +771,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -765,7 +807,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="6"/>
@@ -790,72 +832,76 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+    </row>
+    <row r="12" ht="104.25" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -877,17 +923,17 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
+    <row r="13" ht="44.25" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>34</v>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -909,17 +955,21 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+    <row r="14" ht="117.0" customHeight="1">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>35</v>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -941,17 +991,19 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
+    <row r="15" ht="31.5" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -974,8 +1026,12 @@
       <c r="Z15" s="6"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>

</xml_diff>